<commit_message>
Set up new layout
</commit_message>
<xml_diff>
--- a/layout.xlsx
+++ b/layout.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>Row/Column</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>defaultfolderButton</t>
+  </si>
+  <si>
+    <t>Minimum burst size - ttk.Label</t>
+  </si>
+  <si>
+    <t>Plot burst probability - ttk.Label</t>
   </si>
 </sst>
 </file>
@@ -538,8 +544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,8 +651,12 @@
       <c r="E4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -665,8 +675,12 @@
       <c r="E5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="F5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated to include new file formats
</commit_message>
<xml_diff>
--- a/layout.xlsx
+++ b/layout.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t>Row/Column</t>
   </si>
@@ -47,9 +47,6 @@
     <t>ttk.Button - analyzeButton</t>
   </si>
   <si>
-    <t>loadmedButton - ttk.Button</t>
-  </si>
-  <si>
     <t>self.f2 - ttk.Frame</t>
   </si>
   <si>
@@ -77,9 +74,6 @@
     <t>About - ttk.Label</t>
   </si>
   <si>
-    <t>Load .txt file - ttk.Button</t>
-  </si>
-  <si>
     <t>pdfButton</t>
   </si>
   <si>
@@ -92,9 +86,6 @@
     <t>nextfile - ttk.Button</t>
   </si>
   <si>
-    <t>Loaded file - ttk.Label</t>
-  </si>
-  <si>
     <t>Total licks</t>
   </si>
   <si>
@@ -126,6 +117,18 @@
   </si>
   <si>
     <t>Plot burst probability - ttk.Label</t>
+  </si>
+  <si>
+    <t>loadfileBtn - ttk.Button</t>
+  </si>
+  <si>
+    <t>File Format - ttk.Label</t>
+  </si>
+  <si>
+    <t>Header Rows - ttk.Label</t>
+  </si>
+  <si>
+    <t>ttk.Dropdown</t>
   </si>
 </sst>
 </file>
@@ -221,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -238,6 +241,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,7 +549,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,15 +602,15 @@
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="5" t="s">
@@ -618,19 +622,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>5</v>
@@ -641,21 +645,23 @@
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="7"/>
+      <c r="B4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="D4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H4" s="5"/>
     </row>
@@ -663,12 +669,10 @@
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="B5" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="7"/>
       <c r="D5" s="2" t="s">
         <v>1</v>
       </c>
@@ -676,7 +680,7 @@
         <v>2</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>5</v>
@@ -687,6 +691,12 @@
       <c r="A6" s="2">
         <v>4</v>
       </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="D6" s="2" t="s">
         <v>3</v>
       </c>
@@ -702,7 +712,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -719,22 +729,22 @@
         <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -742,7 +752,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -793,7 +803,7 @@
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:H6"/>
-    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -815,32 +825,32 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>